<commit_message>
second round of corrections
</commit_message>
<xml_diff>
--- a/publication/supplements/S1_plasmodium_benchmark.xlsx
+++ b/publication/supplements/S1_plasmodium_benchmark.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="S1_plasmodium_benchmark" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>H</t>
   </si>
@@ -85,52 +85,46 @@
     <t>MCC</t>
   </si>
   <si>
-    <t>signalHsmm</t>
-  </si>
-  <si>
     <t>Software</t>
   </si>
   <si>
-    <t>Predsi</t>
-  </si>
-  <si>
     <t>Philius</t>
   </si>
   <si>
     <t>Phobius</t>
   </si>
   <si>
-    <t>SignalP 4.1. (no tm)</t>
-  </si>
-  <si>
-    <t>SignalP 4.1. (tm)</t>
-  </si>
-  <si>
-    <t>SignalP 3.0 (NN)</t>
-  </si>
-  <si>
-    <t>SignalP 3.0 (HMM)</t>
-  </si>
-  <si>
-    <t>signalHsmm (homol. red. 50%)</t>
-  </si>
-  <si>
-    <t>signalHsmm (homol. red. 90%)</t>
-  </si>
-  <si>
-    <t>signalHsmm (raw aa)</t>
-  </si>
-  <si>
-    <t>signalHsmm_1987</t>
-  </si>
-  <si>
-    <t>signalHsmm_1987 (raw aa)</t>
-  </si>
-  <si>
-    <t>signalHsmm_1987 (homol. red. 50%)</t>
-  </si>
-  <si>
-    <t>signalHsmm_1987 (homol. red. 90%)</t>
+    <t>signalP 4.1 (no tm)</t>
+  </si>
+  <si>
+    <t>signalP 4.1 (tm)</t>
+  </si>
+  <si>
+    <t>signalP 3.0 (NN)</t>
+  </si>
+  <si>
+    <t>signalP 3.0 (HMM)</t>
+  </si>
+  <si>
+    <t>PrediSi</t>
+  </si>
+  <si>
+    <t>signalHsmm-2010</t>
+  </si>
+  <si>
+    <t>signalHsmm-2010 (homol. red. 50%)</t>
+  </si>
+  <si>
+    <t>signalHsmm-2010 (raw aa)</t>
+  </si>
+  <si>
+    <t>signalHsmm-1987</t>
+  </si>
+  <si>
+    <t>signalHsmm-1987 (homol. red. 50%)</t>
+  </si>
+  <si>
+    <t>signalHsmm-1987 (raw aa)</t>
   </si>
 </sst>
 </file>
@@ -985,18 +979,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X16"/>
+  <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.21875" customWidth="1"/>
     <col min="2" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="19" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.6640625" customWidth="1"/>
+    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3.109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="3" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="4" bestFit="1" customWidth="1"/>
@@ -1004,9 +998,9 @@
     <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1080,120 +1074,120 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2">
-        <v>0.63848000000000005</v>
+        <v>0.61018799999999995</v>
       </c>
       <c r="C2">
-        <v>0.76321899999999998</v>
+        <v>0.73348199999999997</v>
       </c>
       <c r="D2">
-        <v>0.88161</v>
+        <v>0.86674099999999998</v>
       </c>
       <c r="E2">
-        <v>0.88161</v>
+        <v>0.86674099999999998</v>
       </c>
       <c r="F2">
-        <v>0.76321899999999998</v>
+        <v>0.73348199999999997</v>
       </c>
       <c r="G2">
         <v>0.10687000000000001</v>
       </c>
       <c r="H2">
-        <v>7.4237999999999998E-2</v>
+        <v>8.3561999999999997E-2</v>
       </c>
       <c r="I2">
-        <v>0.57244399999999995</v>
+        <v>0.65213299999999996</v>
       </c>
       <c r="J2">
-        <v>0.42931799999999998</v>
+        <v>0.36625400000000002</v>
       </c>
       <c r="K2">
         <v>0.10687000000000001</v>
       </c>
       <c r="L2">
-        <v>0.86274499999999998</v>
+        <v>0.82352899999999996</v>
       </c>
       <c r="M2">
-        <v>0.900474</v>
+        <v>0.90995300000000001</v>
       </c>
       <c r="N2">
-        <v>0.67692300000000005</v>
+        <v>0.68852500000000005</v>
       </c>
       <c r="O2">
-        <v>0.86274499999999998</v>
+        <v>0.82352899999999996</v>
       </c>
       <c r="P2">
-        <v>0.86274499999999998</v>
+        <v>0.82352899999999996</v>
       </c>
       <c r="Q2">
-        <v>9.9526000000000003E-2</v>
+        <v>9.0047000000000002E-2</v>
       </c>
       <c r="R2">
-        <v>0.75862099999999999</v>
+        <v>0.75</v>
       </c>
       <c r="S2">
-        <v>0.76321899999999998</v>
+        <v>0.73348199999999997</v>
       </c>
       <c r="T2">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="U2">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="V2">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="W2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="X2">
-        <v>0.699658</v>
+        <v>0.68715199999999999</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1">
-        <v>0.46492800000000001</v>
+        <v>0.47396700000000003</v>
       </c>
       <c r="C3" s="1">
-        <v>0.58544700000000005</v>
+        <v>0.59018700000000002</v>
       </c>
       <c r="D3" s="1">
-        <v>0.79272399999999998</v>
+        <v>0.79509300000000005</v>
       </c>
       <c r="E3" s="1">
-        <v>0.79272399999999998</v>
+        <v>0.79509300000000005</v>
       </c>
       <c r="F3" s="1">
-        <v>0.58544700000000005</v>
+        <v>0.59018700000000002</v>
       </c>
       <c r="G3" s="1">
-        <v>0.118321</v>
+        <v>0.11450399999999999</v>
       </c>
       <c r="H3" s="1">
-        <v>0.12997500000000001</v>
+        <v>0.12848899999999999</v>
       </c>
       <c r="I3" s="1">
-        <v>0.80545</v>
+        <v>0.80951799999999996</v>
       </c>
       <c r="J3" s="1">
-        <v>0.121946</v>
+        <v>7.8186000000000005E-2</v>
       </c>
       <c r="K3" s="1">
-        <v>0.118321</v>
+        <v>0.11450399999999999</v>
       </c>
       <c r="L3" s="1">
         <v>0.64705900000000005</v>
       </c>
       <c r="M3" s="1">
-        <v>0.93838900000000003</v>
+        <v>0.94312799999999997</v>
       </c>
       <c r="N3" s="1">
-        <v>0.717391</v>
+        <v>0.73333300000000001</v>
       </c>
       <c r="O3" s="1">
         <v>0.64705900000000005</v>
@@ -1202,33 +1196,33 @@
         <v>0.64705900000000005</v>
       </c>
       <c r="Q3" s="1">
-        <v>6.1610999999999999E-2</v>
+        <v>5.6871999999999999E-2</v>
       </c>
       <c r="R3" s="1">
-        <v>0.68041200000000002</v>
+        <v>0.6875</v>
       </c>
       <c r="S3" s="1">
-        <v>0.58544700000000005</v>
+        <v>0.59018700000000002</v>
       </c>
       <c r="T3" s="1">
         <v>33</v>
       </c>
       <c r="U3" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V3" s="1">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="W3" s="1">
         <v>18</v>
       </c>
       <c r="X3" s="1">
-        <v>0.60926800000000003</v>
+        <v>0.61955499999999997</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>0.67093100000000006</v>
@@ -1302,81 +1296,81 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1">
-        <v>0.30136499999999999</v>
+        <v>0.40840599999999999</v>
       </c>
       <c r="C5" s="1">
-        <v>0.55450200000000005</v>
+        <v>0.54688199999999998</v>
       </c>
       <c r="D5" s="1">
-        <v>0.77725100000000003</v>
+        <v>0.77344100000000005</v>
       </c>
       <c r="E5" s="1">
-        <v>0.77725100000000003</v>
+        <v>0.77344100000000005</v>
       </c>
       <c r="F5" s="1">
-        <v>0.55450200000000005</v>
+        <v>0.54688199999999998</v>
       </c>
       <c r="G5" s="1">
-        <v>0.194656</v>
+        <v>0.137405</v>
       </c>
       <c r="H5" s="1">
-        <v>0.139677</v>
+        <v>0.142066</v>
       </c>
       <c r="I5" s="1">
-        <v>0.97772499999999996</v>
+        <v>0.79603400000000002</v>
       </c>
       <c r="J5" s="1">
-        <v>0.88776600000000006</v>
+        <v>0.238062</v>
       </c>
       <c r="K5" s="1">
-        <v>0.35877900000000001</v>
+        <v>0.137405</v>
       </c>
       <c r="L5" s="1">
-        <v>1</v>
+        <v>0.62745099999999998</v>
       </c>
       <c r="M5" s="1">
-        <v>0.55450200000000005</v>
+        <v>0.919431</v>
       </c>
       <c r="N5" s="1">
-        <v>0.35172399999999998</v>
+        <v>0.653061</v>
       </c>
       <c r="O5" s="1">
-        <v>1</v>
+        <v>0.62745099999999998</v>
       </c>
       <c r="P5" s="1">
-        <v>1</v>
+        <v>0.62745099999999998</v>
       </c>
       <c r="Q5" s="1">
-        <v>0.44549800000000001</v>
+        <v>8.0569000000000002E-2</v>
       </c>
       <c r="R5" s="1">
-        <v>0.52040799999999998</v>
+        <v>0.64</v>
       </c>
       <c r="S5" s="1">
-        <v>0.55450200000000005</v>
+        <v>0.54688199999999998</v>
       </c>
       <c r="T5" s="1">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="U5" s="1">
-        <v>94</v>
+        <v>17</v>
       </c>
       <c r="V5" s="1">
-        <v>117</v>
+        <v>194</v>
       </c>
       <c r="W5" s="1">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="X5" s="1">
-        <v>0.44162400000000002</v>
+        <v>0.55530599999999997</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>0.191522</v>
@@ -1450,7 +1444,7 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1">
         <v>0.41406199999999999</v>
@@ -1524,7 +1518,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>0.44700000000000001</v>
@@ -1598,298 +1592,298 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1">
-        <v>0.74533799999999995</v>
+        <v>0.72654399999999997</v>
       </c>
       <c r="C9" s="1">
-        <v>0.87436100000000005</v>
+        <v>0.85243000000000002</v>
       </c>
       <c r="D9" s="1">
-        <v>0.93718100000000004</v>
+        <v>0.92621500000000001</v>
       </c>
       <c r="E9" s="1">
-        <v>0.94549799999999995</v>
+        <v>0.92621500000000001</v>
       </c>
       <c r="F9" s="1">
-        <v>0.86729900000000004</v>
+        <v>0.85243000000000002</v>
       </c>
       <c r="G9" s="1">
         <v>0.10687000000000001</v>
       </c>
       <c r="H9" s="1">
-        <v>4.1605999999999997E-2</v>
+        <v>4.6267999999999997E-2</v>
       </c>
       <c r="I9" s="1">
+        <v>0.99603299999999995</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.59731299999999998</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.10687000000000001</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.98039200000000004</v>
+      </c>
+      <c r="M9" s="1">
         <v>0.87203799999999998</v>
       </c>
-      <c r="J9" s="1">
-        <v>0.31372499999999998</v>
-      </c>
-      <c r="K9" s="1">
-        <v>0.194656</v>
-      </c>
-      <c r="L9" s="1">
+      <c r="N9" s="1">
+        <v>0.64935100000000001</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0.98039200000000004</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0.98039200000000004</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0.12796199999999999</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0.78125</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0.85243000000000002</v>
+      </c>
+      <c r="T9" s="1">
+        <v>50</v>
+      </c>
+      <c r="U9" s="1">
+        <v>27</v>
+      </c>
+      <c r="V9" s="1">
+        <v>184</v>
+      </c>
+      <c r="W9" s="1">
         <v>1</v>
       </c>
-      <c r="M9" s="1">
-        <v>0.75829400000000002</v>
-      </c>
-      <c r="N9" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="O9" s="1">
-        <v>1</v>
-      </c>
-      <c r="P9" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>0.241706</v>
-      </c>
-      <c r="R9" s="1">
-        <v>0.66666700000000001</v>
-      </c>
-      <c r="S9" s="1">
-        <v>0.75829400000000002</v>
-      </c>
-      <c r="T9" s="1">
-        <v>51</v>
-      </c>
-      <c r="U9" s="1">
-        <v>51</v>
-      </c>
-      <c r="V9" s="1">
-        <v>160</v>
-      </c>
-      <c r="W9" s="1">
-        <v>0</v>
-      </c>
       <c r="X9" s="1">
-        <v>0.61574899999999999</v>
+        <v>0.74089000000000005</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10">
-        <v>0.68851499999999999</v>
+        <v>0.75930799999999998</v>
       </c>
       <c r="C10">
-        <v>0.84313700000000003</v>
+        <v>0.87677700000000003</v>
       </c>
       <c r="D10">
-        <v>0.92156899999999997</v>
+        <v>0.93838900000000003</v>
       </c>
       <c r="E10">
-        <v>0.93490399999999996</v>
+        <v>0.93838900000000003</v>
       </c>
       <c r="F10">
-        <v>0.80912600000000001</v>
+        <v>0.87677700000000003</v>
       </c>
       <c r="G10">
-        <v>0.10687000000000001</v>
+        <v>9.9237000000000006E-2</v>
       </c>
       <c r="H10">
-        <v>5.9845000000000002E-2</v>
+        <v>3.8634000000000002E-2</v>
       </c>
       <c r="I10">
-        <v>0.84834100000000001</v>
+        <v>0.99383900000000003</v>
       </c>
       <c r="J10">
-        <v>0.39215699999999998</v>
+        <v>0.59423099999999995</v>
       </c>
       <c r="K10">
-        <v>0.24045800000000001</v>
+        <v>9.9237000000000006E-2</v>
       </c>
       <c r="L10">
-        <v>0.96078399999999997</v>
+        <v>1</v>
       </c>
       <c r="M10">
-        <v>0.71089999999999998</v>
+        <v>0.87677700000000003</v>
       </c>
       <c r="N10">
-        <v>0.44545499999999999</v>
+        <v>0.66233799999999998</v>
       </c>
       <c r="O10">
-        <v>0.96078399999999997</v>
+        <v>1</v>
       </c>
       <c r="P10">
-        <v>0.96078399999999997</v>
+        <v>1</v>
       </c>
       <c r="Q10">
-        <v>0.28910000000000002</v>
+        <v>0.123223</v>
       </c>
       <c r="R10">
-        <v>0.60869600000000001</v>
+        <v>0.796875</v>
       </c>
       <c r="S10">
-        <v>0.67168499999999998</v>
+        <v>0.87677700000000003</v>
       </c>
       <c r="T10">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="U10">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="V10">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="W10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X10">
-        <v>0.53885700000000003</v>
+        <v>0.76205199999999995</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1">
-        <v>0.76020799999999999</v>
+        <v>0.61524800000000002</v>
       </c>
       <c r="C11" s="1">
-        <v>0.87417500000000004</v>
+        <v>0.74361100000000002</v>
       </c>
       <c r="D11" s="1">
-        <v>0.93708800000000003</v>
+        <v>0.87180599999999997</v>
       </c>
       <c r="E11" s="1">
-        <v>0.94572999999999996</v>
+        <v>0.87180599999999997</v>
       </c>
       <c r="F11" s="1">
-        <v>0.87677700000000003</v>
+        <v>0.74361100000000002</v>
       </c>
       <c r="G11" s="1">
-        <v>9.9237000000000006E-2</v>
+        <v>0.11068699999999999</v>
       </c>
       <c r="H11" s="1">
-        <v>3.8634000000000002E-2</v>
+        <v>8.0385999999999999E-2</v>
       </c>
       <c r="I11" s="1">
-        <v>0.87677700000000003</v>
+        <v>0.61344799999999999</v>
       </c>
       <c r="J11" s="1">
-        <v>0.31372499999999998</v>
+        <v>0.41956100000000002</v>
       </c>
       <c r="K11" s="1">
-        <v>0.22137399999999999</v>
+        <v>0.11068699999999999</v>
       </c>
       <c r="L11" s="1">
-        <v>1</v>
+        <v>0.84313700000000003</v>
       </c>
       <c r="M11" s="1">
-        <v>0.72511800000000004</v>
+        <v>0.900474</v>
       </c>
       <c r="N11" s="1">
-        <v>0.46788999999999997</v>
+        <v>0.671875</v>
       </c>
       <c r="O11" s="1">
-        <v>1</v>
+        <v>0.84313700000000003</v>
       </c>
       <c r="P11" s="1">
-        <v>1</v>
+        <v>0.84313700000000003</v>
       </c>
       <c r="Q11" s="1">
-        <v>0.27488200000000002</v>
+        <v>9.9526000000000003E-2</v>
       </c>
       <c r="R11" s="1">
-        <v>0.63749999999999996</v>
+        <v>0.74782599999999999</v>
       </c>
       <c r="S11" s="1">
-        <v>0.72511800000000004</v>
+        <v>0.74361100000000002</v>
       </c>
       <c r="T11" s="1">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="U11" s="1">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="V11" s="1">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="W11" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X11" s="1">
-        <v>0.58247400000000005</v>
+        <v>0.68525100000000005</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12">
-        <v>0.74619100000000005</v>
+        <v>0.69100300000000003</v>
       </c>
       <c r="C12">
-        <v>0.87082999999999999</v>
+        <v>0.81256399999999995</v>
       </c>
       <c r="D12">
-        <v>0.935415</v>
+        <v>0.90628200000000003</v>
       </c>
       <c r="E12">
-        <v>0.94401100000000004</v>
+        <v>0.90628200000000003</v>
       </c>
       <c r="F12">
-        <v>0.86729900000000004</v>
+        <v>0.81256399999999995</v>
       </c>
       <c r="G12">
         <v>0.10305300000000001</v>
       </c>
       <c r="H12">
-        <v>4.1605999999999997E-2</v>
+        <v>5.8767E-2</v>
       </c>
       <c r="I12">
-        <v>0.87677700000000003</v>
+        <v>0.322986</v>
       </c>
       <c r="J12">
-        <v>0.31372499999999998</v>
+        <v>0.49884899999999999</v>
       </c>
       <c r="K12">
-        <v>0.19847300000000001</v>
+        <v>0.10305300000000001</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>0.92156899999999997</v>
       </c>
       <c r="M12">
-        <v>0.75355499999999997</v>
+        <v>0.89099499999999998</v>
       </c>
       <c r="N12">
-        <v>0.49514599999999998</v>
+        <v>0.67142900000000005</v>
       </c>
       <c r="O12">
-        <v>1</v>
+        <v>0.92156899999999997</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>0.92156899999999997</v>
       </c>
       <c r="Q12">
-        <v>0.246445</v>
+        <v>0.109005</v>
       </c>
       <c r="R12">
-        <v>0.66233799999999998</v>
+        <v>0.77685999999999999</v>
       </c>
       <c r="S12">
-        <v>0.75355499999999997</v>
+        <v>0.81256399999999995</v>
       </c>
       <c r="T12">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="U12">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="V12">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="W12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X12">
-        <v>0.61083500000000002</v>
+        <v>0.72708300000000003</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
@@ -1897,73 +1891,73 @@
         <v>35</v>
       </c>
       <c r="B13" s="1">
-        <v>0.71012600000000003</v>
+        <v>0.68788700000000003</v>
       </c>
       <c r="C13" s="1">
-        <v>0.87120200000000003</v>
+        <v>0.81795399999999996</v>
       </c>
       <c r="D13" s="1">
-        <v>0.93560100000000002</v>
+        <v>0.90897700000000003</v>
       </c>
       <c r="E13" s="1">
-        <v>0.94689199999999996</v>
+        <v>0.90897700000000003</v>
       </c>
       <c r="F13" s="1">
-        <v>0.818604</v>
+        <v>0.81795399999999996</v>
       </c>
       <c r="G13" s="1">
-        <v>9.5420000000000005E-2</v>
+        <v>0.11068699999999999</v>
       </c>
       <c r="H13" s="1">
-        <v>5.6873E-2</v>
+        <v>5.7077000000000003E-2</v>
       </c>
       <c r="I13" s="1">
-        <v>0.85782000000000003</v>
+        <v>0.131517</v>
       </c>
       <c r="J13" s="1">
-        <v>0.41176499999999999</v>
+        <v>0.559276</v>
       </c>
       <c r="K13" s="1">
-        <v>0.16412199999999999</v>
+        <v>0.11068699999999999</v>
       </c>
       <c r="L13" s="1">
-        <v>0.96078399999999997</v>
+        <v>0.94117600000000001</v>
       </c>
       <c r="M13" s="1">
-        <v>0.80568700000000004</v>
+        <v>0.87677700000000003</v>
       </c>
       <c r="N13" s="1">
-        <v>0.54444400000000004</v>
+        <v>0.64864900000000003</v>
       </c>
       <c r="O13" s="1">
-        <v>0.96078399999999997</v>
+        <v>0.94117600000000001</v>
       </c>
       <c r="P13" s="1">
-        <v>0.96078399999999997</v>
+        <v>0.94117600000000001</v>
       </c>
       <c r="Q13" s="1">
-        <v>0.19431300000000001</v>
+        <v>0.123223</v>
       </c>
       <c r="R13" s="1">
-        <v>0.69503499999999996</v>
+        <v>0.76800000000000002</v>
       </c>
       <c r="S13" s="1">
-        <v>0.76647200000000004</v>
+        <v>0.81795399999999996</v>
       </c>
       <c r="T13" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U13" s="1">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="V13" s="1">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="W13" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X13" s="1">
-        <v>0.63905299999999998</v>
+        <v>0.71938299999999999</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
@@ -1971,221 +1965,73 @@
         <v>36</v>
       </c>
       <c r="B14">
-        <v>0.693774</v>
+        <v>0.53310100000000005</v>
       </c>
       <c r="C14">
-        <v>0.84295100000000001</v>
+        <v>0.66991900000000004</v>
       </c>
       <c r="D14">
-        <v>0.92147599999999996</v>
+        <v>0.83496000000000004</v>
       </c>
       <c r="E14">
-        <v>0.93471800000000005</v>
+        <v>0.83496000000000004</v>
       </c>
       <c r="F14">
-        <v>0.81795399999999996</v>
+        <v>0.66991900000000004</v>
       </c>
       <c r="G14">
-        <v>0.11068699999999999</v>
+        <v>0.122137</v>
       </c>
       <c r="H14">
-        <v>5.7077000000000003E-2</v>
+        <v>0.10349</v>
       </c>
       <c r="I14">
-        <v>0.85308099999999998</v>
+        <v>0.71285500000000002</v>
       </c>
       <c r="J14">
-        <v>0.43137300000000001</v>
+        <v>0.36132399999999998</v>
       </c>
       <c r="K14">
-        <v>0.15648899999999999</v>
+        <v>0.122137</v>
       </c>
       <c r="L14">
-        <v>0.96078399999999997</v>
+        <v>0.764706</v>
       </c>
       <c r="M14">
-        <v>0.81516599999999995</v>
+        <v>0.90521300000000005</v>
       </c>
       <c r="N14">
-        <v>0.55681800000000004</v>
+        <v>0.66101699999999997</v>
       </c>
       <c r="O14">
-        <v>0.96078399999999997</v>
+        <v>0.764706</v>
       </c>
       <c r="P14">
-        <v>0.96078399999999997</v>
+        <v>0.764706</v>
       </c>
       <c r="Q14">
-        <v>0.184834</v>
+        <v>9.4786999999999996E-2</v>
       </c>
       <c r="R14">
-        <v>0.705036</v>
+        <v>0.70909100000000003</v>
       </c>
       <c r="S14">
-        <v>0.77595000000000003</v>
+        <v>0.66991900000000004</v>
       </c>
       <c r="T14">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="U14">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="V14">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="W14">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="X14">
-        <v>0.65049500000000005</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="1">
-        <v>0.71256900000000001</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0.87157300000000004</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.93578700000000004</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0.94679899999999995</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0.83282199999999995</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0.10687000000000001</v>
-      </c>
-      <c r="H15" s="1">
-        <v>5.2415000000000003E-2</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0.87203799999999998</v>
-      </c>
-      <c r="J15" s="1">
-        <v>0.45097999999999999</v>
-      </c>
-      <c r="K15" s="1">
-        <v>0.167939</v>
-      </c>
-      <c r="L15" s="1">
-        <v>0.98039200000000004</v>
-      </c>
-      <c r="M15" s="1">
-        <v>0.79620899999999994</v>
-      </c>
-      <c r="N15" s="1">
-        <v>0.53763399999999995</v>
-      </c>
-      <c r="O15" s="1">
-        <v>0.98039200000000004</v>
-      </c>
-      <c r="P15" s="1">
-        <v>0.98039200000000004</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>0.203791</v>
-      </c>
-      <c r="R15" s="1">
-        <v>0.69444399999999995</v>
-      </c>
-      <c r="S15" s="1">
-        <v>0.77660099999999999</v>
-      </c>
-      <c r="T15" s="1">
-        <v>50</v>
-      </c>
-      <c r="U15" s="1">
-        <v>43</v>
-      </c>
-      <c r="V15" s="1">
-        <v>168</v>
-      </c>
-      <c r="W15" s="1">
-        <v>1</v>
-      </c>
-      <c r="X15" s="1">
-        <v>0.642598</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16">
-        <v>0.718445</v>
-      </c>
-      <c r="C16">
-        <v>0.87138700000000002</v>
-      </c>
-      <c r="D16">
-        <v>0.93569400000000003</v>
-      </c>
-      <c r="E16">
-        <v>0.94652000000000003</v>
-      </c>
-      <c r="F16">
-        <v>0.82808300000000001</v>
-      </c>
-      <c r="G16">
-        <v>9.5420000000000005E-2</v>
-      </c>
-      <c r="H16">
-        <v>5.3900999999999998E-2</v>
-      </c>
-      <c r="I16">
-        <v>0.86729900000000004</v>
-      </c>
-      <c r="J16">
-        <v>0.43137300000000001</v>
-      </c>
-      <c r="K16">
-        <v>0.16412199999999999</v>
-      </c>
-      <c r="L16">
-        <v>0.96078399999999997</v>
-      </c>
-      <c r="M16">
-        <v>0.80568700000000004</v>
-      </c>
-      <c r="N16">
-        <v>0.54444400000000004</v>
-      </c>
-      <c r="O16">
-        <v>0.96078399999999997</v>
-      </c>
-      <c r="P16">
-        <v>0.96078399999999997</v>
-      </c>
-      <c r="Q16">
-        <v>0.19431300000000001</v>
-      </c>
-      <c r="R16">
-        <v>0.69503499999999996</v>
-      </c>
-      <c r="S16">
-        <v>0.76647200000000004</v>
-      </c>
-      <c r="T16">
-        <v>49</v>
-      </c>
-      <c r="U16">
-        <v>41</v>
-      </c>
-      <c r="V16">
-        <v>170</v>
-      </c>
-      <c r="W16">
-        <v>2</v>
-      </c>
-      <c r="X16">
-        <v>0.63905299999999998</v>
+        <v>0.63500100000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>